<commit_message>
[200~HW123 MPU6050, I2C connection attempted. Not yet successful, errors present.
</commit_message>
<xml_diff>
--- a/link_Komunikation.xlsx
+++ b/link_Komunikation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emrah\OneDrive\Desktop\Photonic Studium\5. Semester 2025 - 2026\Prototyping\Projekt_Prototyping_HS25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22ce4f5b18f5d7de/Desktop/Photonic Studium/5. Semester 2025 - 2026/Prototyping/Projekt_Prototyping_HS25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555E3EE4-B5E8-4EF7-B220-105842362BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{555E3EE4-B5E8-4EF7-B220-105842362BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E144A826-2B9E-4DB7-AB54-A9B0DE34E8CF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">FireBeetle Mikrokontroller info: </t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>DFRobot ESP32 and Arduino Tutorial List: Everything You Need to Know - DFRobot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPU I2C: </t>
+  </si>
+  <si>
+    <t>Arduino Guide for MPU-6050 Accelerometer and Gyroscope | Random Nerd Tutorials</t>
   </si>
 </sst>
 </file>
@@ -83,10 +89,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -371,20 +377,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:J7"/>
+  <dimension ref="B6:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
@@ -394,12 +400,20 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -410,6 +424,7 @@
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" display="https://wiki.dfrobot.com/FireBeetle_Board_ESP32_E_SKU_DFR0654" xr:uid="{59E31F01-D267-4937-8C40-F9F536396184}"/>
     <hyperlink ref="D7" r:id="rId2" display="https://www.dfrobot.com/blog-1578.html" xr:uid="{96753300-627C-42E7-A9F4-DC5BCA3304C0}"/>
+    <hyperlink ref="C9" r:id="rId3" display="https://randomnerdtutorials.com/arduino-mpu-6050-accelerometer-gyroscope/" xr:uid="{A1EF1C0D-7E39-49DD-929C-6D5A765B8BC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Foto und Fusion wurde entwickelt
</commit_message>
<xml_diff>
--- a/link_Komunikation.xlsx
+++ b/link_Komunikation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22ce4f5b18f5d7de/Desktop/Photonic Studium/5. Semester 2025 - 2026/Prototyping/Projekt_Prototyping_HS25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{555E3EE4-B5E8-4EF7-B220-105842362BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E144A826-2B9E-4DB7-AB54-A9B0DE34E8CF}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{555E3EE4-B5E8-4EF7-B220-105842362BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23FC5EE4-B37A-41D3-B7D6-42E6A21D8CCA}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">FireBeetle Mikrokontroller info: </t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Arduino Guide for MPU-6050 Accelerometer and Gyroscope | Random Nerd Tutorials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LearnPortal: </t>
+  </si>
+  <si>
+    <t>ESP32 MPU-6050 Accelerometer and Gyroscope (Arduino) | Random Nerd Tutorials</t>
   </si>
 </sst>
 </file>
@@ -112,6 +118,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,15 +387,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:J9"/>
+  <dimension ref="B6:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -400,7 +410,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -408,12 +418,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -425,6 +443,7 @@
     <hyperlink ref="E6" r:id="rId1" display="https://wiki.dfrobot.com/FireBeetle_Board_ESP32_E_SKU_DFR0654" xr:uid="{59E31F01-D267-4937-8C40-F9F536396184}"/>
     <hyperlink ref="D7" r:id="rId2" display="https://www.dfrobot.com/blog-1578.html" xr:uid="{96753300-627C-42E7-A9F4-DC5BCA3304C0}"/>
     <hyperlink ref="C9" r:id="rId3" display="https://randomnerdtutorials.com/arduino-mpu-6050-accelerometer-gyroscope/" xr:uid="{A1EF1C0D-7E39-49DD-929C-6D5A765B8BC4}"/>
+    <hyperlink ref="D11" r:id="rId4" display="https://randomnerdtutorials.com/esp32-mpu-6050-accelerometer-gyroscope-arduino/" xr:uid="{FBD255C4-76AA-4408-9354-0B2AC34B300F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>